<commit_message>
Create Account TC is completed
</commit_message>
<xml_diff>
--- a/src/main/java/resources/AuthenTeak_TestData.xlsx
+++ b/src/main/java/resources/AuthenTeak_TestData.xlsx
@@ -50,12 +50,6 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>abctest</t>
-  </si>
-  <si>
     <t>India</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>abc1234</t>
+  </si>
+  <si>
+    <t>abc2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -491,34 +491,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
       </c>
       <c r="K2">
         <v>411045</v>

</xml_diff>